<commit_message>
deixando as cores das planilhas padronizadas, de acordo com as cores do nosso site institucional
</commit_message>
<xml_diff>
--- a/documentacao/Dicionário de Dados.xlsx
+++ b/documentacao/Dicionário de Dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Facul BandTec\PI\Projeto PI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\blind-market\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -275,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +291,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9797"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,18 +398,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,22 +434,46 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -460,6 +484,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9797"/>
       <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
@@ -740,7 +765,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,202 +810,202 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="23">
         <v>50</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="23">
         <v>50</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="18">
         <v>50</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="18">
         <v>50</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -993,7 +1018,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,92 +1062,92 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="18">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="18">
         <v>50</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1134,7 +1159,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,52 +1203,52 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="18">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1235,7 +1260,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,82 +1304,82 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1368,7 +1393,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B3" sqref="B3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,62 +1437,62 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="18">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="22" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1481,7 +1506,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,82 +1550,82 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="24">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="25" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="27">
         <v>5.2</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="30" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizando cores das planilhas novamente
</commit_message>
<xml_diff>
--- a/documentacao/Dicionário de Dados.xlsx
+++ b/documentacao/Dicionário de Dados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\blind-market\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\blind-market\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="DD EMPRESA" sheetId="1" r:id="rId1"/>
@@ -296,13 +296,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF9797"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9797"/>
+        <fgColor rgb="FFFF8F8F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,9 +441,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,22 +458,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +472,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,19 +813,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -833,19 +833,19 @@
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="30">
         <v>50</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="30" t="s">
         <v>23</v>
       </c>
     </row>
@@ -853,19 +853,19 @@
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="30">
         <v>50</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="30" t="s">
         <v>24</v>
       </c>
     </row>
@@ -873,19 +873,19 @@
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="25">
         <v>50</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -893,19 +893,19 @@
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="25">
         <v>50</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1065,19 +1065,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1085,19 +1085,19 @@
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="25">
         <v>50</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1105,19 +1105,19 @@
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="25">
         <v>50</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1125,19 +1125,19 @@
       <c r="A6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,19 +1206,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1226,19 +1226,19 @@
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="25">
         <v>50</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1307,19 +1307,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1327,19 +1327,19 @@
       <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1347,19 +1347,19 @@
       <c r="A5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="26" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1367,19 +1367,19 @@
       <c r="A6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="26" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,19 +1440,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="25">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1460,19 +1460,19 @@
       <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="25">
         <v>50</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="27" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1480,19 +1480,19 @@
       <c r="A5" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="29" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1505,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,19 +1553,19 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1573,19 +1573,19 @@
       <c r="A4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1593,19 +1593,19 @@
       <c r="A5" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="21">
         <v>5.2</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1613,19 +1613,19 @@
       <c r="A6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="24" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizando as cores das planilhas mais uma vez
</commit_message>
<xml_diff>
--- a/documentacao/Dicionário de Dados.xlsx
+++ b/documentacao/Dicionário de Dados.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="DD EMPRESA" sheetId="1" r:id="rId1"/>
-    <sheet name="DD ESTABELECIMENTO" sheetId="2" r:id="rId2"/>
+    <sheet name="DD ESTABELECIMENTO" sheetId="2" r:id="rId1"/>
+    <sheet name="DD EMPRESA" sheetId="1" r:id="rId2"/>
     <sheet name="DD Categoria" sheetId="3" r:id="rId3"/>
     <sheet name="DD REGISTRO" sheetId="4" r:id="rId4"/>
     <sheet name="DDSENSOR" sheetId="5" r:id="rId5"/>
@@ -251,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,8 +274,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,18 +311,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9797"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8F8F"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -334,10 +343,10 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
@@ -350,7 +359,55 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
@@ -358,16 +415,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="1"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -375,8 +430,126 @@
       <left style="thin">
         <color theme="1"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color theme="1"/>
@@ -388,28 +561,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,53 +584,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,8 +664,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF5050"/>
       <color rgb="FFFF9797"/>
-      <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -762,395 +942,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="30" t="s">
+      <c r="F3" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="9">
         <v>50</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="30" t="s">
+      <c r="F4" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="9">
         <v>50</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="25">
-        <v>50</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="25">
-        <v>50</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F5" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="25" t="s">
+      <c r="F3" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="31">
         <v>50</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="25" t="s">
+      <c r="F4" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="31">
         <v>50</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="F5" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9">
+        <v>50</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="29">
+        <v>50</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1159,96 +1339,96 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="29">
         <v>50</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1266,120 +1446,120 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="30" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1393,106 +1573,106 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B3" sqref="B3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="9">
         <v>50</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1505,127 +1685,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="9">
         <v>4</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="11">
         <v>5.2</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="28" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>